<commit_message>
excel tambah mitra di survei sudah ada validasinya
</commit_message>
<xml_diff>
--- a/kito/public/addMitra2Survey.xlsx
+++ b/kito/public/addMitra2Survey.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mag\project mitra\MitraBPS\ProjekMitraBPS\kito\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RIZKY\Documents\magang\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4E7AFB7-5E7C-40B6-908A-72C51B995E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7190"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,21 +25,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>id_mitra</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>posisi</t>
   </si>
   <si>
-    <t>contoh</t>
+    <t>sobat_id</t>
+  </si>
+  <si>
+    <t>contoh999</t>
+  </si>
+  <si>
+    <t>tahun_mitra</t>
+  </si>
+  <si>
+    <t>S003</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -349,29 +356,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="C1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>2</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
+      </c>
+      <c r="C2">
+        <v>2025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update template excel addmitra
</commit_message>
<xml_diff>
--- a/kito/public/addMitra2Survey.xlsx
+++ b/kito/public/addMitra2Survey.xlsx
@@ -1,30 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mag\project mitra\MitraBPS\ProjekMitraBPS\kito\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rizky\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F7B570-5497-4FEC-A7AB-9B11CD122BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7190"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>posisi</t>
   </si>
@@ -42,12 +52,6 @@
   </si>
   <si>
     <t>vol</t>
-  </si>
-  <si>
-    <t>rate_honor</t>
-  </si>
-  <si>
-    <t>100000</t>
   </si>
   <si>
     <t>5</t>
@@ -74,7 +78,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -110,11 +114,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -152,7 +155,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{45D2D6F2-E293-BCA7-870D-51D0886E5B55}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45D2D6F2-E293-BCA7-870D-51D0886E5B55}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -504,71 +507,65 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="8.90625" style="1"/>
-    <col min="7" max="7" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.81640625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="6" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>6</v>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update import mitra ke survei
</commit_message>
<xml_diff>
--- a/kito/public/addMitra2Survey.xlsx
+++ b/kito/public/addMitra2Survey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rizky\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F7B570-5497-4FEC-A7AB-9B11CD122BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E06E03-FB5B-4497-B12F-8E6C712F2343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>posisi</t>
   </si>
@@ -42,9 +42,6 @@
     <t>sobat_id</t>
   </si>
   <si>
-    <t>tgl_ikut_survei</t>
-  </si>
-  <si>
     <t>catatan</t>
   </si>
   <si>
@@ -70,9 +67,6 @@
   </si>
   <si>
     <t>15-03-2018</t>
-  </si>
-  <si>
-    <t>11-11-1991</t>
   </si>
 </sst>
 </file>
@@ -147,8 +141,8 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>487680</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>31750</xdr:rowOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -163,8 +157,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6531610" y="53340"/>
-          <a:ext cx="1671320" cy="3293110"/>
+          <a:off x="6400800" y="53340"/>
+          <a:ext cx="1645920" cy="1722120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -219,22 +213,11 @@
           </a:pPr>
           <a:r>
             <a:rPr lang="id-ID" sz="1100" b="1" baseline="0"/>
-            <a:t>tgl_ikut_survei jika tidak di isi maka akan otomatis berisi tanggal </a:t>
+            <a:t>catatan dan nilai sebaiknya di isi jika status survei sudah dikerjakan</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t>hari ini</a:t>
-          </a:r>
-          <a:endParaRPr lang="id-ID" sz="1100" b="1" baseline="0"/>
-        </a:p>
-        <a:p>
-          <a:pPr marL="171450" indent="-171450" algn="l">
-            <a:buFont typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:buChar char="•"/>
-          </a:pPr>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100" b="1" baseline="0"/>
-            <a:t>catatan dan nilai sebaiknya di isi jika status survei sudah dikerjakan</a:t>
+            <a:t>, agar tidak usah mengisi manual satu satu</a:t>
           </a:r>
           <a:endParaRPr lang="id-ID" sz="1100" b="1"/>
         </a:p>
@@ -508,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,7 +505,7 @@
     <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -530,42 +513,36 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update manual input mitra ke survei dan template nya
</commit_message>
<xml_diff>
--- a/kito/public/addMitra2Survey.xlsx
+++ b/kito/public/addMitra2Survey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rizky\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E06E03-FB5B-4497-B12F-8E6C712F2343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06ECAA74-B0EA-4C08-818D-92001B5C2706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>posisi</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>15-03-2018</t>
+  </si>
+  <si>
+    <t>rate_honor</t>
   </si>
 </sst>
 </file>
@@ -491,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -505,7 +508,7 @@
     <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -515,17 +518,20 @@
       <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -536,12 +542,15 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>